<commit_message>
all test case complete
</commit_message>
<xml_diff>
--- a/Numbers.xlsx
+++ b/Numbers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQA Projects\QUPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQA Projects\QUPS\Whatsapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBD6F24-D990-46E4-8C97-BD48A046CED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F00EB1D-2C3C-4DB3-8519-167A09061706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="16770" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
-  <si>
-    <t>Phone Number</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+  <si>
+    <t>Phone Numbers</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Message Status</t>
   </si>
   <si>
     <t>Sent</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Delivered </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sent </t>
+  </si>
+  <si>
+    <t>not seen</t>
   </si>
 </sst>
 </file>
@@ -47,12 +62,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -69,7 +90,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,7 +371,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -358,25 +379,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1771176464</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
all test case done
</commit_message>
<xml_diff>
--- a/Numbers.xlsx
+++ b/Numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQA Projects\QUPS\Whatsapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F00EB1D-2C3C-4DB3-8519-167A09061706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB43CE4-8122-460C-BCDA-7616D4F5D4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="16770" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t>Phone Numbers</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>Sent</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Delivered </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sent </t>
   </si>
   <si>
     <t>not seen</t>
@@ -374,7 +368,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,7 +397,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all test case working properly
</commit_message>
<xml_diff>
--- a/Numbers.xlsx
+++ b/Numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQA Projects\QUPS\Whatsapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB43CE4-8122-460C-BCDA-7616D4F5D4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063AF7C7-D1E4-4167-8FBC-CECB3A85BA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="16770" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="765" yWindow="2040" windowWidth="16770" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Phone Numbers</t>
   </si>

</xml_diff>